<commit_message>
Beginning of yearly incidence rate
</commit_message>
<xml_diff>
--- a/Data/brca_incidence_2004_17.xlsx
+++ b/Data/brca_incidence_2004_17.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Google Drive (pp10001@cam.ac.uk)/Teaching/MPhil/AppliedDataAnalysis/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelkoll/Desktop/4/Masters/c/Course/ADA/Practical/Breast-cancer-incidence-analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639A1F2E-6651-BB4B-89D1-E092511DC72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A3ACF7-D0CC-1542-B198-0A6E53E9B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24400" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
@@ -133,13 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11618,15 +11617,15 @@
   <dimension ref="A3:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11692,49 +11691,49 @@
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5">
         <v>0</v>
       </c>
     </row>
@@ -11742,49 +11741,49 @@
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6">
         <v>0</v>
       </c>
     </row>
@@ -11792,49 +11791,49 @@
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7">
         <v>0</v>
       </c>
     </row>
@@ -11842,49 +11841,49 @@
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8">
         <v>0</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8">
         <v>0</v>
       </c>
     </row>
@@ -11892,49 +11891,49 @@
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9">
         <v>0</v>
       </c>
     </row>
@@ -11942,49 +11941,49 @@
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10">
         <v>11</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10">
         <v>7</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10">
         <v>6</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10">
         <v>29</v>
       </c>
     </row>
@@ -11992,49 +11991,49 @@
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>6</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>14</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>9</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <v>13</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <v>19</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <v>27</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11">
         <v>12</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11">
         <v>15</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11">
         <v>31</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>17</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11">
         <v>22</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11">
         <v>12</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11">
         <v>27</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11">
         <v>240</v>
       </c>
     </row>
@@ -12042,49 +12041,49 @@
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>46</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>53</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>47</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>51</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>61</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <v>51</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <v>51</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12">
         <v>30</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12">
         <v>44</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12">
         <v>55</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12">
         <v>33</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12">
         <v>46</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12">
         <v>58</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12">
         <v>48</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12">
         <v>674</v>
       </c>
     </row>
@@ -12092,49 +12091,49 @@
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>96</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>90</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>114</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <v>100</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <v>98</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>118</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13">
         <v>106</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13">
         <v>105</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13">
         <v>109</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13">
         <v>113</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13">
         <v>79</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13">
         <v>98</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13">
         <v>103</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13">
         <v>110</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13">
         <v>1439</v>
       </c>
     </row>
@@ -12142,49 +12141,49 @@
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>133</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>136</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>152</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>145</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>153</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <v>162</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14">
         <v>159</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14">
         <v>193</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14">
         <v>205</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14">
         <v>263</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14">
         <v>243</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14">
         <v>182</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14">
         <v>181</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14">
         <v>165</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14">
         <v>2472</v>
       </c>
     </row>
@@ -12192,49 +12191,49 @@
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>209</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>211</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>231</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>208</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>235</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15">
         <v>228</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <v>206</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15">
         <v>225</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15">
         <v>205</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15">
         <v>207</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15">
         <v>260</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15">
         <v>231</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15">
         <v>234</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15">
         <v>226</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15">
         <v>3116</v>
       </c>
     </row>
@@ -12242,49 +12241,49 @@
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>222</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>236</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>223</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>203</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>163</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16">
         <v>208</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16">
         <v>203</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16">
         <v>206</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16">
         <v>190</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16">
         <v>192</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16">
         <v>217</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16">
         <v>200</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16">
         <v>246</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16">
         <v>211</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16">
         <v>2920</v>
       </c>
     </row>
@@ -12292,49 +12291,49 @@
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>211</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>285</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>205</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>194</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>294</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17">
         <v>356</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17">
         <v>304</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17">
         <v>262</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17">
         <v>284</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17">
         <v>252</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17">
         <v>268</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17">
         <v>258</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17">
         <v>220</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17">
         <v>241</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17">
         <v>3634</v>
       </c>
     </row>
@@ -12342,49 +12341,49 @@
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>293</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>180</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>206</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>249</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>275</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <v>237</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18">
         <v>252</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18">
         <v>313</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18">
         <v>325</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18">
         <v>322</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>347</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M18">
         <v>392</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18">
         <v>370</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18">
         <v>300</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18">
         <v>4061</v>
       </c>
     </row>
@@ -12392,49 +12391,49 @@
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>193</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>144</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>173</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>158</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>168</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>131</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19">
         <v>163</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19">
         <v>178</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19">
         <v>164</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19">
         <v>181</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19">
         <v>219</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19">
         <v>227</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19">
         <v>216</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19">
         <v>256</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19">
         <v>2571</v>
       </c>
     </row>
@@ -12442,49 +12441,49 @@
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>155</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>168</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20">
         <v>159</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>152</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <v>196</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20">
         <v>186</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20">
         <v>185</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20">
         <v>196</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20">
         <v>185</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20">
         <v>207</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20">
         <v>200</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20">
         <v>186</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20">
         <v>206</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20">
         <v>218</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20">
         <v>2599</v>
       </c>
     </row>
@@ -12492,49 +12491,49 @@
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21">
         <v>171</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>145</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21">
         <v>148</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>136</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <v>142</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21">
         <v>161</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21">
         <v>152</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21">
         <v>154</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21">
         <v>162</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21">
         <v>158</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21">
         <v>195</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21">
         <v>183</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21">
         <v>166</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21">
         <v>181</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21">
         <v>2254</v>
       </c>
     </row>
@@ -12542,49 +12541,49 @@
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>76</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>84</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22">
         <v>78</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>102</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <v>106</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22">
         <v>127</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22">
         <v>109</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22">
         <v>119</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22">
         <v>110</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22">
         <v>125</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22">
         <v>129</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22">
         <v>142</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22">
         <v>105</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22">
         <v>137</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22">
         <v>1549</v>
       </c>
     </row>
@@ -12592,49 +12591,49 @@
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>46</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23">
         <v>49</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23">
         <v>51</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>59</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <v>59</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23">
         <v>51</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23">
         <v>73</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23">
         <v>66</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23">
         <v>67</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23">
         <v>75</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23">
         <v>92</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23">
         <v>92</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23">
         <v>77</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23">
         <v>73</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23">
         <v>930</v>
       </c>
     </row>
@@ -12642,49 +12641,49 @@
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>1872</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24">
         <v>1787</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24">
         <v>1801</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>1766</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24">
         <v>1963</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24">
         <v>2035</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24">
         <v>1990</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24">
         <v>2059</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24">
         <v>2076</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24">
         <v>2181</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24">
         <v>2299</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24">
         <v>2266</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24">
         <v>2200</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24">
         <v>2193</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24">
         <v>28488</v>
       </c>
     </row>

</xml_diff>